<commit_message>
corrected error in wgs overview
</commit_message>
<xml_diff>
--- a/apps/template_docs/Antibiotics.xlsx
+++ b/apps/template_docs/Antibiotics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CEL_PROJECT_home\REFERRED_DB_090425\REFERRED_DB\apps\template_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\REFERRED_DB_052325\REFERRED_DB\apps\template_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DCE0E5E2-50E7-44F2-83A8-C1C1ECCE62DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450BAB8C-6930-4D74-AF23-D96F7BF3C5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antibiotics" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,23 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Antibiotics!$E$1:$L$164</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2130" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="733">
   <si>
     <t>CLSI</t>
   </si>
@@ -2169,12 +2180,66 @@
   </si>
   <si>
     <t>CBX_NM</t>
+  </si>
+  <si>
+    <t>BooleanField</t>
+  </si>
+  <si>
+    <t>DateField</t>
+  </si>
+  <si>
+    <t>default=True</t>
+  </si>
+  <si>
+    <t>auto_now_add=True</t>
+  </si>
+  <si>
+    <t>max_length=100, blank=True, default=''''</t>
+  </si>
+  <si>
+    <t>Show=models.BooleanField(default=True)</t>
+  </si>
+  <si>
+    <t>Retest=models.BooleanField(default=True)</t>
+  </si>
+  <si>
+    <t>Disk_Abx=models.BooleanField(default=True)</t>
+  </si>
+  <si>
+    <t>Date_Modified=models.DateField(auto_now_add=True)</t>
+  </si>
+  <si>
+    <t>Test_Method=models.Charfield(max_length=100, blank=True, default="")</t>
+  </si>
+  <si>
+    <t>Abx_Code=models.Charfield(max_length=100, blank=True, default="")</t>
+  </si>
+  <si>
+    <t>Whonet_Abx=models.Charfield(max_length=100, blank=True, default="")</t>
+  </si>
+  <si>
+    <t>Antibiotic=models.Charfield(max_length=100, blank=True, default="")</t>
+  </si>
+  <si>
+    <t>Guidelines=models.Charfield(max_length=100, blank=True, default="")</t>
+  </si>
+  <si>
+    <t>Potency=models.Charfield(max_length=100, blank=True, default="")</t>
+  </si>
+  <si>
+    <t>Class=models.Charfield(max_length=100, blank=True, default="")</t>
+  </si>
+  <si>
+    <t>Subclass=models.Charfield(max_length=100, blank=True, default="")</t>
+  </si>
+  <si>
+    <t>CharField</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2673,13 +2738,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3034,11 +3105,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L327"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13468,7 +13539,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:L164"/>
+  <autoFilter ref="E1:L164" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L327">
     <sortCondition ref="F1:F327"/>
   </sortState>
@@ -13478,15 +13549,238 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="68.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="B1" t="s">
+        <v>715</v>
+      </c>
+      <c r="C1" t="s">
+        <v>717</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE(A1,"=","models.",B1,"(",C1,")","")</f>
+        <v>Show=models.BooleanField(default=True)</v>
+      </c>
+      <c r="E1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="B2" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2" t="s">
+        <v>717</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D12" si="0">CONCATENATE(A2,"=","models.",B2,"(",C2,")","")</f>
+        <v>Retest=models.BooleanField(default=True)</v>
+      </c>
+      <c r="E2" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="B3" t="s">
+        <v>715</v>
+      </c>
+      <c r="C3" t="s">
+        <v>717</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>Disk_Abx=models.BooleanField(default=True)</v>
+      </c>
+      <c r="E3" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="B4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C4" t="s">
+        <v>719</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>Test_Method=models.CharField(max_length=100, blank=True, default='''')</v>
+      </c>
+      <c r="E4" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="B5" t="s">
+        <v>732</v>
+      </c>
+      <c r="C5" t="s">
+        <v>719</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>Abx_Code=models.CharField(max_length=100, blank=True, default='''')</v>
+      </c>
+      <c r="E5" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B6" t="s">
+        <v>732</v>
+      </c>
+      <c r="C6" t="s">
+        <v>719</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>Whonet_Abx=models.CharField(max_length=100, blank=True, default='''')</v>
+      </c>
+      <c r="E6" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>549</v>
+      </c>
+      <c r="B7" t="s">
+        <v>732</v>
+      </c>
+      <c r="C7" t="s">
+        <v>719</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>Antibiotic=models.CharField(max_length=100, blank=True, default='''')</v>
+      </c>
+      <c r="E7" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>550</v>
+      </c>
+      <c r="B8" t="s">
+        <v>732</v>
+      </c>
+      <c r="C8" t="s">
+        <v>719</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>Guidelines=models.CharField(max_length=100, blank=True, default='''')</v>
+      </c>
+      <c r="E8" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="B9" t="s">
+        <v>732</v>
+      </c>
+      <c r="C9" t="s">
+        <v>719</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>Potency=models.CharField(max_length=100, blank=True, default='''')</v>
+      </c>
+      <c r="E9" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="B10" t="s">
+        <v>732</v>
+      </c>
+      <c r="C10" t="s">
+        <v>719</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>Class=models.CharField(max_length=100, blank=True, default='''')</v>
+      </c>
+      <c r="E10" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>553</v>
+      </c>
+      <c r="B11" t="s">
+        <v>732</v>
+      </c>
+      <c r="C11" t="s">
+        <v>719</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>Subclass=models.CharField(max_length=100, blank=True, default='''')</v>
+      </c>
+      <c r="E11" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="B12" t="s">
+        <v>716</v>
+      </c>
+      <c r="C12" t="s">
+        <v>718</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>Date_Modified=models.DateField(auto_now_add=True)</v>
+      </c>
+      <c r="E12" t="s">
+        <v>723</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>